<commit_message>
Updating weights and quality scores
</commit_message>
<xml_diff>
--- a/config/weights/Metadata-Quality-Weights.xlsx
+++ b/config/weights/Metadata-Quality-Weights.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/susheel/DATA/code/src/github.com/hdruk/datasets/config/weights/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85361D94-FC12-3B43-BE20-B5995A82DD2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E3B36E-FA80-EB4C-BC7E-DF83C0AE3848}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9200" yWindow="-28340" windowWidth="51200" windowHeight="28340" activeTab="3" xr2:uid="{995D6B0F-EEA3-1C47-AA4E-15299B43967E}"/>
+    <workbookView xWindow="-9200" yWindow="-28340" windowWidth="25600" windowHeight="28340" activeTab="2" xr2:uid="{995D6B0F-EEA3-1C47-AA4E-15299B43967E}"/>
   </bookViews>
   <sheets>
     <sheet name="V1 V2 Mapping" sheetId="1" r:id="rId1"/>
@@ -1034,7 +1034,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1154,12 +1154,6 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1167,6 +1161,14 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1490,8 +1492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA6A415A-4C4C-344F-9CF3-865979E84061}">
   <dimension ref="A1:L84"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4:K83"/>
+    <sheetView topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30:K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1511,18 +1513,18 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:12" s="1" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="93" t="s">
+      <c r="B2" s="100" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="94"/>
+      <c r="C2" s="101"/>
       <c r="D2" s="31"/>
       <c r="E2" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="G2" s="93" t="s">
+      <c r="G2" s="100" t="s">
         <v>91</v>
       </c>
-      <c r="H2" s="94"/>
+      <c r="H2" s="101"/>
       <c r="I2" s="66"/>
       <c r="K2" s="78" t="s">
         <v>150</v>
@@ -1557,7 +1559,7 @@
       </c>
       <c r="K4" s="76">
         <f>SUM(K5:K22)</f>
-        <v>0.20567375886524819</v>
+        <v>0.19463087248322145</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
@@ -1588,7 +1590,7 @@
       </c>
       <c r="K5" s="70">
         <f t="shared" ref="K5:K22" si="0">J5/$J$84</f>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
@@ -1619,7 +1621,7 @@
       </c>
       <c r="K6" s="72">
         <f t="shared" si="0"/>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
@@ -1650,7 +1652,7 @@
       </c>
       <c r="K7" s="72">
         <f t="shared" si="0"/>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
@@ -1681,7 +1683,7 @@
       </c>
       <c r="K8" s="72">
         <f t="shared" si="0"/>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
@@ -1712,7 +1714,7 @@
       </c>
       <c r="K9" s="72">
         <f t="shared" si="0"/>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
@@ -1772,7 +1774,7 @@
       </c>
       <c r="K11" s="72">
         <f t="shared" si="0"/>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="12" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1828,7 +1830,7 @@
       </c>
       <c r="K13" s="72">
         <f t="shared" si="0"/>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.2">
@@ -1941,7 +1943,7 @@
       </c>
       <c r="K17" s="72">
         <f t="shared" si="0"/>
-        <v>7.0921985815602835E-3</v>
+        <v>6.7114093959731542E-3</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
@@ -2122,7 +2124,7 @@
       <c r="J24" s="30"/>
       <c r="K24" s="76">
         <f>SUM(K25:K27)</f>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
@@ -2152,7 +2154,7 @@
       </c>
       <c r="K25" s="70">
         <f>J25/$J$84</f>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="26" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2240,7 +2242,7 @@
       <c r="J29" s="30"/>
       <c r="K29" s="76">
         <f>SUM(K30:K34)</f>
-        <v>8.5106382978723402E-2</v>
+        <v>9.3959731543624164E-2</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.2">
@@ -2270,7 +2272,7 @@
       </c>
       <c r="K30" s="70">
         <f>J30/$J$84</f>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.2">
@@ -2301,7 +2303,7 @@
       </c>
       <c r="K31" s="72">
         <f>J31/$J$84</f>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
@@ -2332,7 +2334,7 @@
       </c>
       <c r="K32" s="72">
         <f>J32/$J$84</f>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="33" spans="2:11" ht="18" x14ac:dyDescent="0.2">
@@ -2348,19 +2350,19 @@
       <c r="G33" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="H33" s="95">
+      <c r="H33" s="93">
         <v>0</v>
       </c>
       <c r="I33" s="71" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J33" s="30">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K33" s="72">
         <f>J33/$J$84</f>
-        <v>0</v>
+        <v>6.7114093959731542E-3</v>
       </c>
     </row>
     <row r="34" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2376,19 +2378,19 @@
       <c r="G34" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="H34" s="96">
+      <c r="H34" s="94">
         <v>0</v>
       </c>
       <c r="I34" s="73" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J34" s="74">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K34" s="75">
         <f>J34/$J$84</f>
-        <v>0</v>
+        <v>6.7114093959731542E-3</v>
       </c>
     </row>
     <row r="35" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2422,7 +2424,7 @@
       <c r="J36" s="30"/>
       <c r="K36" s="76">
         <f>SUM(K37:K44)</f>
-        <v>5.6737588652482268E-2</v>
+        <v>8.0536912751677861E-2</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
@@ -2443,15 +2445,15 @@
         <v>0</v>
       </c>
       <c r="I37" s="68" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J37" s="69">
         <f>IF(I37="MAN",4,IF(I37="REQ",1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K37" s="70">
         <f t="shared" ref="K37:K44" si="4">J37/$J$84</f>
-        <v>0</v>
+        <v>6.7114093959731542E-3</v>
       </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.2">
@@ -2472,15 +2474,15 @@
         <v>0</v>
       </c>
       <c r="I38" s="71" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J38" s="30">
         <f t="shared" ref="J38:J44" si="5">IF(I38="MAN",4,IF(I38="REQ",1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K38" s="72">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6.7114093959731542E-3</v>
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
@@ -2501,15 +2503,15 @@
         <v>0</v>
       </c>
       <c r="I39" s="71" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J39" s="30">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K39" s="72">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6.7114093959731542E-3</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
@@ -2539,7 +2541,7 @@
       </c>
       <c r="K40" s="72">
         <f t="shared" si="4"/>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
@@ -2599,7 +2601,7 @@
       </c>
       <c r="K42" s="72">
         <f t="shared" si="4"/>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="43" spans="2:11" ht="18" x14ac:dyDescent="0.2">
@@ -2632,19 +2634,19 @@
       <c r="G44" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="H44" s="96">
+      <c r="H44" s="94">
         <v>1.5873016E-2</v>
       </c>
       <c r="I44" s="73" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J44" s="74">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K44" s="75">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6.7114093959731542E-3</v>
       </c>
     </row>
     <row r="45" spans="2:11" ht="19" thickBot="1" x14ac:dyDescent="0.25">
@@ -2677,7 +2679,7 @@
       <c r="J46" s="30"/>
       <c r="K46" s="76">
         <f>SUM(K47:K62)</f>
-        <v>0.34751773049645379</v>
+        <v>0.34228187919463088</v>
       </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.2">
@@ -2694,7 +2696,7 @@
       <c r="G47" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="H47" s="95">
+      <c r="H47" s="93">
         <f>C34</f>
         <v>1.5873016E-2</v>
       </c>
@@ -2707,7 +2709,7 @@
       </c>
       <c r="K47" s="70">
         <f t="shared" ref="K47:K62" si="6">J47/$J$84</f>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.2">
@@ -2724,7 +2726,7 @@
       <c r="G48" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="H48" s="95">
+      <c r="H48" s="93">
         <f>C35</f>
         <v>1.5873016E-2</v>
       </c>
@@ -2737,7 +2739,7 @@
       </c>
       <c r="K48" s="72">
         <f t="shared" si="6"/>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.2">
@@ -2767,7 +2769,7 @@
       </c>
       <c r="K49" s="72">
         <f t="shared" si="6"/>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="50" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2782,19 +2784,19 @@
       <c r="G50" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="H50" s="95">
+      <c r="H50" s="93">
         <v>0</v>
       </c>
       <c r="I50" s="71" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J50" s="30">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K50" s="72">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>6.7114093959731542E-3</v>
       </c>
     </row>
     <row r="51" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2812,15 +2814,15 @@
         <v>1.5873016E-2</v>
       </c>
       <c r="I51" s="71" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J51" s="30">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K51" s="72">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>6.7114093959731542E-3</v>
       </c>
     </row>
     <row r="52" spans="2:11" ht="19" thickBot="1" x14ac:dyDescent="0.25">
@@ -2851,7 +2853,7 @@
       </c>
       <c r="K52" s="72">
         <f t="shared" si="6"/>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.2">
@@ -2868,7 +2870,7 @@
       <c r="G53" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="H53" s="95">
+      <c r="H53" s="93">
         <v>1.5873016E-2</v>
       </c>
       <c r="I53" s="71" t="s">
@@ -2880,7 +2882,7 @@
       </c>
       <c r="K53" s="72">
         <f t="shared" si="6"/>
-        <v>7.0921985815602835E-3</v>
+        <v>6.7114093959731542E-3</v>
       </c>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.2">
@@ -2910,7 +2912,7 @@
       </c>
       <c r="K54" s="72">
         <f t="shared" si="6"/>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="55" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2940,7 +2942,7 @@
       </c>
       <c r="K55" s="72">
         <f t="shared" si="6"/>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="56" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2966,7 +2968,7 @@
       </c>
       <c r="K56" s="72">
         <f t="shared" si="6"/>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="57" spans="2:11" ht="19" thickBot="1" x14ac:dyDescent="0.25">
@@ -2996,7 +2998,7 @@
       </c>
       <c r="K57" s="72">
         <f t="shared" si="6"/>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.2">
@@ -3054,7 +3056,7 @@
       </c>
       <c r="K59" s="72">
         <f t="shared" si="6"/>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.2">
@@ -3083,7 +3085,7 @@
       </c>
       <c r="K60" s="72">
         <f t="shared" si="6"/>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.2">
@@ -3112,7 +3114,7 @@
       </c>
       <c r="K61" s="72">
         <f t="shared" si="6"/>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="62" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3125,10 +3127,10 @@
       <c r="E62" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="G62" s="100" t="s">
+      <c r="G62" s="98" t="s">
         <v>108</v>
       </c>
-      <c r="H62" s="97">
+      <c r="H62" s="95">
         <f>C49</f>
         <v>1.5873016E-2</v>
       </c>
@@ -3141,7 +3143,7 @@
       </c>
       <c r="K62" s="75">
         <f t="shared" si="6"/>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="63" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3172,7 +3174,7 @@
       <c r="J64" s="30"/>
       <c r="K64" s="76">
         <f>SUM(K65:K67)</f>
-        <v>2.1276595744680851E-2</v>
+        <v>2.0134228187919462E-2</v>
       </c>
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.2">
@@ -3187,7 +3189,7 @@
       <c r="G65" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="H65" s="98">
+      <c r="H65" s="96">
         <f>C24</f>
         <v>3.1746032E-2</v>
       </c>
@@ -3200,7 +3202,7 @@
       </c>
       <c r="K65" s="70">
         <f>J65/$J$84</f>
-        <v>7.0921985815602835E-3</v>
+        <v>6.7114093959731542E-3</v>
       </c>
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.2">
@@ -3223,7 +3225,7 @@
       </c>
       <c r="K66" s="72">
         <f>J66/$J$84</f>
-        <v>7.0921985815602835E-3</v>
+        <v>6.7114093959731542E-3</v>
       </c>
     </row>
     <row r="67" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3231,7 +3233,7 @@
       <c r="G67" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="H67" s="96">
+      <c r="H67" s="94">
         <v>0</v>
       </c>
       <c r="I67" s="73" t="s">
@@ -3243,7 +3245,7 @@
       </c>
       <c r="K67" s="75">
         <f>J67/$J$84</f>
-        <v>7.0921985815602835E-3</v>
+        <v>6.7114093959731542E-3</v>
       </c>
     </row>
     <row r="68" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3260,17 +3262,17 @@
       <c r="J69" s="30"/>
       <c r="K69" s="76">
         <f>SUM(K70:K74)</f>
-        <v>5.6737588652482268E-2</v>
+        <v>5.3691275167785234E-2</v>
       </c>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.2">
       <c r="E70" s="88" t="s">
         <v>151</v>
       </c>
-      <c r="G70" s="101" t="s">
+      <c r="G70" s="99" t="s">
         <v>85</v>
       </c>
-      <c r="H70" s="99">
+      <c r="H70" s="97">
         <v>0</v>
       </c>
       <c r="I70" s="68" t="s">
@@ -3282,7 +3284,7 @@
       </c>
       <c r="K70" s="70">
         <f>J70/$J$84</f>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.2">
@@ -3292,7 +3294,7 @@
       <c r="G71" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="H71" s="95">
+      <c r="H71" s="93">
         <v>0</v>
       </c>
       <c r="I71" s="71" t="s">
@@ -3304,7 +3306,7 @@
       </c>
       <c r="K71" s="72">
         <f>J71/$J$84</f>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.2">
@@ -3312,7 +3314,7 @@
       <c r="G72" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="H72" s="95">
+      <c r="H72" s="93">
         <v>0</v>
       </c>
       <c r="I72" s="71" t="s">
@@ -3332,7 +3334,7 @@
       <c r="G73" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="H73" s="95">
+      <c r="H73" s="93">
         <v>0</v>
       </c>
       <c r="I73" s="71" t="s">
@@ -3352,7 +3354,7 @@
       <c r="G74" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="H74" s="96">
+      <c r="H74" s="94">
         <v>0</v>
       </c>
       <c r="I74" s="73" t="s">
@@ -3381,7 +3383,7 @@
       <c r="J76" s="30"/>
       <c r="K76" s="76">
         <f>SUM(K77:K83)</f>
-        <v>0.1985815602836879</v>
+        <v>0.1879194630872483</v>
       </c>
     </row>
     <row r="77" spans="2:11" x14ac:dyDescent="0.2">
@@ -3404,7 +3406,7 @@
       </c>
       <c r="K77" s="70">
         <f t="shared" ref="K77:K83" si="11">J77/$J$84</f>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="78" spans="2:11" x14ac:dyDescent="0.2">
@@ -3427,7 +3429,7 @@
       </c>
       <c r="K78" s="72">
         <f t="shared" si="11"/>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="79" spans="2:11" x14ac:dyDescent="0.2">
@@ -3450,7 +3452,7 @@
       </c>
       <c r="K79" s="72">
         <f t="shared" si="11"/>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="80" spans="2:11" x14ac:dyDescent="0.2">
@@ -3473,7 +3475,7 @@
       </c>
       <c r="K80" s="72">
         <f t="shared" si="11"/>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="81" spans="5:11" x14ac:dyDescent="0.2">
@@ -3496,7 +3498,7 @@
       </c>
       <c r="K81" s="72">
         <f t="shared" si="11"/>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="82" spans="5:11" x14ac:dyDescent="0.2">
@@ -3519,7 +3521,7 @@
       </c>
       <c r="K82" s="72">
         <f t="shared" si="11"/>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="83" spans="5:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3529,7 +3531,7 @@
       <c r="G83" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="H83" s="97">
+      <c r="H83" s="95">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -3542,7 +3544,7 @@
       </c>
       <c r="K83" s="75">
         <f t="shared" si="11"/>
-        <v>2.8368794326241134E-2</v>
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="84" spans="5:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3553,7 +3555,7 @@
       </c>
       <c r="J84" s="1">
         <f>SUM(J5:J83)</f>
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -4054,15 +4056,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64A232B5-B804-F542-A152-E639116A203C}">
   <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60:C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.83203125" customWidth="1"/>
-    <col min="3" max="3" width="31" customWidth="1"/>
+    <col min="3" max="3" width="31" style="102" customWidth="1"/>
     <col min="4" max="4" width="13.5" customWidth="1"/>
     <col min="5" max="5" width="11.83203125" customWidth="1"/>
   </cols>
@@ -4074,7 +4076,7 @@
       <c r="B1" t="s">
         <v>94</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="102" t="s">
         <v>97</v>
       </c>
     </row>
@@ -4085,8 +4087,8 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>2.8368794326241134E-2</v>
+      <c r="C2" s="102">
+        <v>2.6845637583892617E-2</v>
       </c>
       <c r="E2" s="65"/>
     </row>
@@ -4097,8 +4099,8 @@
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3">
-        <v>2.8368794326241134E-2</v>
+      <c r="C3" s="102">
+        <v>2.6845637583892617E-2</v>
       </c>
       <c r="E3" s="65"/>
     </row>
@@ -4109,8 +4111,8 @@
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4">
-        <v>2.8368794326241134E-2</v>
+      <c r="C4" s="102">
+        <v>2.6845637583892617E-2</v>
       </c>
       <c r="E4" s="65"/>
     </row>
@@ -4121,8 +4123,8 @@
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5">
-        <v>2.8368794326241134E-2</v>
+      <c r="C5" s="102">
+        <v>2.6845637583892617E-2</v>
       </c>
       <c r="E5" s="65"/>
     </row>
@@ -4133,8 +4135,8 @@
       <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="C6">
-        <v>2.8368794326241134E-2</v>
+      <c r="C6" s="102">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -4144,7 +4146,7 @@
       <c r="B7" t="s">
         <v>33</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="102">
         <v>0</v>
       </c>
     </row>
@@ -4155,8 +4157,8 @@
       <c r="B8" t="s">
         <v>156</v>
       </c>
-      <c r="C8">
-        <v>2.8368794326241134E-2</v>
+      <c r="C8" s="102">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -4166,7 +4168,7 @@
       <c r="B9" s="65" t="s">
         <v>159</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="102">
         <v>0</v>
       </c>
     </row>
@@ -4177,8 +4179,8 @@
       <c r="B10" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="C10">
-        <v>2.8368794326241134E-2</v>
+      <c r="C10" s="102">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -4188,7 +4190,7 @@
       <c r="B11" s="65" t="s">
         <v>157</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="102">
         <v>0</v>
       </c>
     </row>
@@ -4199,7 +4201,7 @@
       <c r="B12" s="65" t="s">
         <v>158</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="102">
         <v>0</v>
       </c>
     </row>
@@ -4210,7 +4212,7 @@
       <c r="B13" s="65" t="s">
         <v>160</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="102">
         <v>0</v>
       </c>
     </row>
@@ -4221,8 +4223,8 @@
       <c r="B14" s="56" t="s">
         <v>155</v>
       </c>
-      <c r="C14">
-        <v>7.0921985815602835E-3</v>
+      <c r="C14" s="102">
+        <v>6.7114093959731542E-3</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -4232,7 +4234,7 @@
       <c r="B15" s="56" t="s">
         <v>161</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="102">
         <v>0</v>
       </c>
     </row>
@@ -4243,7 +4245,7 @@
       <c r="B16" s="56" t="s">
         <v>162</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="102">
         <v>0</v>
       </c>
     </row>
@@ -4254,7 +4256,7 @@
       <c r="B17" s="56" t="s">
         <v>163</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="102">
         <v>0</v>
       </c>
     </row>
@@ -4265,7 +4267,7 @@
       <c r="B18" s="56" t="s">
         <v>164</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="102">
         <v>0</v>
       </c>
     </row>
@@ -4276,7 +4278,7 @@
       <c r="B19" s="56" t="s">
         <v>165</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="102">
         <v>0</v>
       </c>
     </row>
@@ -4287,8 +4289,8 @@
       <c r="B20" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="C20">
-        <v>2.8368794326241134E-2</v>
+      <c r="C20" s="102">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -4298,7 +4300,7 @@
       <c r="B21" s="65" t="s">
         <v>143</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="102">
         <v>0</v>
       </c>
     </row>
@@ -4309,7 +4311,7 @@
       <c r="B22" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="102">
         <v>0</v>
       </c>
     </row>
@@ -4320,8 +4322,8 @@
       <c r="B23" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="65">
-        <v>2.8368794326241134E-2</v>
+      <c r="C23" s="103">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -4331,8 +4333,8 @@
       <c r="B24" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="C24">
-        <v>2.8368794326241134E-2</v>
+      <c r="C24" s="102">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -4342,8 +4344,8 @@
       <c r="B25" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="C25">
-        <v>2.8368794326241134E-2</v>
+      <c r="C25" s="102">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -4353,8 +4355,8 @@
       <c r="B26" s="56" t="s">
         <v>120</v>
       </c>
-      <c r="C26" s="65">
-        <v>0</v>
+      <c r="C26" s="103">
+        <v>6.7114093959731542E-3</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -4364,8 +4366,8 @@
       <c r="B27" s="56" t="s">
         <v>121</v>
       </c>
-      <c r="C27" s="65">
-        <v>0</v>
+      <c r="C27" s="103">
+        <v>6.7114093959731542E-3</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -4375,8 +4377,8 @@
       <c r="B28" s="65" t="s">
         <v>122</v>
       </c>
-      <c r="C28">
-        <v>0</v>
+      <c r="C28" s="102">
+        <v>6.7114093959731542E-3</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -4386,8 +4388,8 @@
       <c r="B29" s="65" t="s">
         <v>123</v>
       </c>
-      <c r="C29">
-        <v>0</v>
+      <c r="C29" s="102">
+        <v>6.7114093959731542E-3</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -4397,8 +4399,8 @@
       <c r="B30" s="65" t="s">
         <v>140</v>
       </c>
-      <c r="C30" s="65">
-        <v>0</v>
+      <c r="C30" s="103">
+        <v>6.7114093959731542E-3</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -4408,8 +4410,8 @@
       <c r="B31" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="65">
-        <v>2.8368794326241134E-2</v>
+      <c r="C31" s="103">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -4419,7 +4421,7 @@
       <c r="B32" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="65">
+      <c r="C32" s="103">
         <v>0</v>
       </c>
     </row>
@@ -4430,8 +4432,8 @@
       <c r="B33" s="65" t="s">
         <v>117</v>
       </c>
-      <c r="C33" s="65">
-        <v>2.8368794326241134E-2</v>
+      <c r="C33" s="103">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -4441,7 +4443,7 @@
       <c r="B34" s="65" t="s">
         <v>118</v>
       </c>
-      <c r="C34" s="65">
+      <c r="C34" s="103">
         <v>0</v>
       </c>
     </row>
@@ -4452,8 +4454,8 @@
       <c r="B35" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="C35">
-        <v>0</v>
+      <c r="C35" s="102">
+        <v>6.7114093959731542E-3</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -4463,8 +4465,8 @@
       <c r="B36" s="65" t="s">
         <v>145</v>
       </c>
-      <c r="C36" s="65">
-        <v>2.8368794326241134E-2</v>
+      <c r="C36" s="103">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -4474,8 +4476,8 @@
       <c r="B37" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="C37">
-        <v>2.8368794326241134E-2</v>
+      <c r="C37" s="102">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -4485,8 +4487,8 @@
       <c r="B38" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="C38" s="65">
-        <v>2.8368794326241134E-2</v>
+      <c r="C38" s="103">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -4496,8 +4498,8 @@
       <c r="B39" s="65" t="s">
         <v>124</v>
       </c>
-      <c r="C39" s="65">
-        <v>0</v>
+      <c r="C39" s="103">
+        <v>6.7114093959731542E-3</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -4507,8 +4509,8 @@
       <c r="B40" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="C40" s="65">
-        <v>0</v>
+      <c r="C40" s="103">
+        <v>6.7114093959731542E-3</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -4518,8 +4520,8 @@
       <c r="B41" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="C41" s="65">
-        <v>2.8368794326241134E-2</v>
+      <c r="C41" s="103">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -4529,8 +4531,8 @@
       <c r="B42" s="65" t="s">
         <v>141</v>
       </c>
-      <c r="C42" s="65">
-        <v>7.0921985815602835E-3</v>
+      <c r="C42" s="103">
+        <v>6.7114093959731542E-3</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -4540,8 +4542,8 @@
       <c r="B43" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="65">
-        <v>2.8368794326241134E-2</v>
+      <c r="C43" s="103">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -4551,8 +4553,8 @@
       <c r="B44" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="C44">
-        <v>2.8368794326241134E-2</v>
+      <c r="C44" s="102">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -4562,8 +4564,8 @@
       <c r="B45" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="C45">
-        <v>2.8368794326241134E-2</v>
+      <c r="C45" s="102">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -4573,8 +4575,8 @@
       <c r="B46" t="s">
         <v>11</v>
       </c>
-      <c r="C46">
-        <v>2.8368794326241134E-2</v>
+      <c r="C46" s="102">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -4584,7 +4586,7 @@
       <c r="B47" t="s">
         <v>12</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="102">
         <v>0</v>
       </c>
     </row>
@@ -4595,8 +4597,8 @@
       <c r="B48" t="s">
         <v>27</v>
       </c>
-      <c r="C48">
-        <v>2.8368794326241134E-2</v>
+      <c r="C48" s="102">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -4606,8 +4608,8 @@
       <c r="B49" t="s">
         <v>26</v>
       </c>
-      <c r="C49">
-        <v>2.8368794326241134E-2</v>
+      <c r="C49" s="102">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -4617,8 +4619,8 @@
       <c r="B50" t="s">
         <v>28</v>
       </c>
-      <c r="C50">
-        <v>2.8368794326241134E-2</v>
+      <c r="C50" s="102">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -4628,8 +4630,8 @@
       <c r="B51" t="s">
         <v>29</v>
       </c>
-      <c r="C51">
-        <v>2.8368794326241134E-2</v>
+      <c r="C51" s="102">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -4639,8 +4641,8 @@
       <c r="B52" t="s">
         <v>15</v>
       </c>
-      <c r="C52">
-        <v>7.0921985815602835E-3</v>
+      <c r="C52" s="102">
+        <v>6.7114093959731542E-3</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -4650,8 +4652,8 @@
       <c r="B53" t="s">
         <v>14</v>
       </c>
-      <c r="C53">
-        <v>7.0921985815602835E-3</v>
+      <c r="C53" s="102">
+        <v>6.7114093959731542E-3</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -4661,8 +4663,8 @@
       <c r="B54" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="C54">
-        <v>7.0921985815602835E-3</v>
+      <c r="C54" s="102">
+        <v>6.7114093959731542E-3</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -4672,8 +4674,8 @@
       <c r="B55" t="s">
         <v>21</v>
       </c>
-      <c r="C55">
-        <v>2.8368794326241134E-2</v>
+      <c r="C55" s="102">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -4683,8 +4685,8 @@
       <c r="B56" t="s">
         <v>22</v>
       </c>
-      <c r="C56">
-        <v>2.8368794326241134E-2</v>
+      <c r="C56" s="102">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -4694,7 +4696,7 @@
       <c r="B57" s="56" t="s">
         <v>126</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="102">
         <v>0</v>
       </c>
     </row>
@@ -4705,7 +4707,7 @@
       <c r="B58" s="56" t="s">
         <v>127</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="102">
         <v>0</v>
       </c>
     </row>
@@ -4716,7 +4718,7 @@
       <c r="B59" s="56" t="s">
         <v>128</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="102">
         <v>0</v>
       </c>
     </row>
@@ -4727,8 +4729,8 @@
       <c r="B60" t="s">
         <v>34</v>
       </c>
-      <c r="C60">
-        <v>2.8368794326241134E-2</v>
+      <c r="C60" s="102">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -4738,8 +4740,8 @@
       <c r="B61" t="s">
         <v>35</v>
       </c>
-      <c r="C61">
-        <v>2.8368794326241134E-2</v>
+      <c r="C61" s="102">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -4749,8 +4751,8 @@
       <c r="B62" t="s">
         <v>36</v>
       </c>
-      <c r="C62">
-        <v>2.8368794326241134E-2</v>
+      <c r="C62" s="102">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -4760,8 +4762,8 @@
       <c r="B63" t="s">
         <v>37</v>
       </c>
-      <c r="C63">
-        <v>2.8368794326241134E-2</v>
+      <c r="C63" s="102">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -4771,8 +4773,8 @@
       <c r="B64" t="s">
         <v>38</v>
       </c>
-      <c r="C64">
-        <v>2.8368794326241134E-2</v>
+      <c r="C64" s="102">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -4782,8 +4784,8 @@
       <c r="B65" t="s">
         <v>39</v>
       </c>
-      <c r="C65">
-        <v>2.8368794326241134E-2</v>
+      <c r="C65" s="102">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -4793,8 +4795,8 @@
       <c r="B66" t="s">
         <v>40</v>
       </c>
-      <c r="C66">
-        <v>2.8368794326241134E-2</v>
+      <c r="C66" s="102">
+        <v>2.6845637583892617E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4808,8 +4810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDAE3C14-E62B-4E42-8D85-5A7A0A1D9816}">
   <dimension ref="B1:F84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4822,14 +4824,14 @@
   <sheetData>
     <row r="1" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:6" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="93" t="s">
+      <c r="B2" s="100" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="94"/>
-      <c r="E2" s="93" t="s">
+      <c r="C2" s="101"/>
+      <c r="E2" s="100" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="94"/>
+      <c r="F2" s="101"/>
     </row>
     <row r="3" spans="2:6" ht="19" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="31"/>
@@ -5618,7 +5620,7 @@
       <c r="C62" s="5">
         <v>4.7619047999999997E-2</v>
       </c>
-      <c r="E62" s="100" t="s">
+      <c r="E62" s="98" t="s">
         <v>108</v>
       </c>
       <c r="F62" s="44">
@@ -5656,7 +5658,7 @@
       <c r="E65" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="F65" s="98">
+      <c r="F65" s="96">
         <v>7.0921985815602835E-3</v>
       </c>
     </row>
@@ -5672,7 +5674,7 @@
       <c r="E67" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="F67" s="96">
+      <c r="F67" s="94">
         <v>7.0921985815602835E-3</v>
       </c>
     </row>
@@ -5686,10 +5688,10 @@
       </c>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E70" s="101" t="s">
+      <c r="E70" s="99" t="s">
         <v>85</v>
       </c>
-      <c r="F70" s="99">
+      <c r="F70" s="97">
         <v>2.8368794326241134E-2</v>
       </c>
     </row>
@@ -5697,7 +5699,7 @@
       <c r="E71" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="F71" s="95">
+      <c r="F71" s="93">
         <v>2.8368794326241134E-2</v>
       </c>
     </row>
@@ -5705,7 +5707,7 @@
       <c r="E72" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="F72" s="95">
+      <c r="F72" s="93">
         <v>0</v>
       </c>
     </row>
@@ -5713,7 +5715,7 @@
       <c r="E73" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="F73" s="95">
+      <c r="F73" s="93">
         <v>0</v>
       </c>
     </row>
@@ -5721,7 +5723,7 @@
       <c r="E74" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F74" s="96">
+      <c r="F74" s="94">
         <v>0</v>
       </c>
     </row>
@@ -5786,7 +5788,7 @@
       <c r="E83" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="F83" s="97">
+      <c r="F83" s="95">
         <v>2.8368794326241134E-2</v>
       </c>
     </row>

</xml_diff>